<commit_message>
Refactor entity alias formation and news pipeline, add Yahoo update script
Optimized entity alias formation with batch alias insertion and in-memory caching for organizations and persons. Refactored news analyzer pipeline to load system prompt from an external file. Improved entity grounding to mark news as grounded only when all symbols and entities are processed. Enhanced REST news collector with new update modes and argument parsing. Added a new script to update both infos and fundamentals from Yahoo Finance, extracting and saving both datasets efficiently. Minor logging and output improvements throughout.
No more prompts in public ;-)
</commit_message>
<xml_diff>
--- a/apps/market_data/not_found_entities.xlsx
+++ b/apps/market_data/not_found_entities.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="156">
   <si>
     <t>name</t>
   </si>
@@ -25,199 +25,463 @@
     <t>role</t>
   </si>
   <si>
-    <t>Docusignto</t>
-  </si>
-  <si>
-    <t>Bakkt Hldgs</t>
-  </si>
-  <si>
-    <t>TVGN-489 T Cell Therapy</t>
-  </si>
-  <si>
-    <t>CPFH Holding Limited</t>
-  </si>
-  <si>
-    <t>NIH-Funded EAP And MN-001 Diabetes Study</t>
-  </si>
-  <si>
-    <t>RLUSD</t>
-  </si>
-  <si>
-    <t>InnovizTwo LiDAR</t>
-  </si>
-  <si>
-    <t>Mike Milotich</t>
-  </si>
-  <si>
-    <t>Eleison Pharmaceuticals</t>
-  </si>
-  <si>
-    <t>NeuroNOS</t>
-  </si>
-  <si>
-    <t>Valour ETPs</t>
-  </si>
-  <si>
-    <t>Swvl Hldgs</t>
-  </si>
-  <si>
-    <t>AiDock</t>
-  </si>
-  <si>
-    <t>The9bit</t>
-  </si>
-  <si>
-    <t>Swaggy Stocks</t>
-  </si>
-  <si>
-    <t>Esousa</t>
-  </si>
-  <si>
-    <t>DualityBio</t>
-  </si>
-  <si>
-    <t>Olenox Energy</t>
-  </si>
-  <si>
-    <t>ChargePoint Hldgs</t>
-  </si>
-  <si>
-    <t>Photonteck</t>
-  </si>
-  <si>
-    <t>UiPathto</t>
-  </si>
-  <si>
-    <t>AVONELLE-X</t>
-  </si>
-  <si>
-    <t>Quanex Building Prods</t>
-  </si>
-  <si>
-    <t>AccessOne Parent Holdings</t>
-  </si>
-  <si>
-    <t>Credilab</t>
-  </si>
-  <si>
-    <t>OX40 antibodies rocatinlimab and amlitelimab</t>
-  </si>
-  <si>
-    <t>Edward Egilinsky</t>
-  </si>
-  <si>
-    <t>chargePoint Hldgs</t>
-  </si>
-  <si>
-    <t>Anaphylm</t>
-  </si>
-  <si>
-    <t>Rafzen</t>
-  </si>
-  <si>
-    <t>Citi TMT Conf</t>
-  </si>
-  <si>
-    <t>Avrideai</t>
-  </si>
-  <si>
-    <t>Kassuuu</t>
-  </si>
-  <si>
-    <t>Citi Global TMT Conf.</t>
-  </si>
-  <si>
-    <t>APVO452</t>
-  </si>
-  <si>
-    <t>APVO451</t>
-  </si>
-  <si>
-    <t>CNM-Au8</t>
-  </si>
-  <si>
-    <t>Orchestra BioMed Hldgs</t>
-  </si>
-  <si>
-    <t>BIIB142</t>
-  </si>
-  <si>
-    <t>Pulmovant</t>
-  </si>
-  <si>
-    <t>RetailPro</t>
-  </si>
-  <si>
-    <t>Hyperscale Data's Ault Markets</t>
-  </si>
-  <si>
-    <t>ThredUpto</t>
-  </si>
-  <si>
-    <t>Biogento</t>
-  </si>
-  <si>
-    <t>Inhabeo</t>
-  </si>
-  <si>
-    <t>Contivue With Susvimo</t>
-  </si>
-  <si>
-    <t>LoveBiome</t>
-  </si>
-  <si>
-    <t>ZenGUARD</t>
-  </si>
-  <si>
-    <t>Warburg Pincus And GTCR Affiliates</t>
-  </si>
-  <si>
-    <t>MOG Digitech</t>
+    <t>HBAR</t>
+  </si>
+  <si>
+    <t>DNKN</t>
+  </si>
+  <si>
+    <t>TSX:DML</t>
+  </si>
+  <si>
+    <t>Insulet Corp</t>
+  </si>
+  <si>
+    <t>Hagerty's Broad Arrow Auctions</t>
+  </si>
+  <si>
+    <t>Audrain Newport Concours &amp; Motor Week</t>
+  </si>
+  <si>
+    <t>Audrain Concours Foundation</t>
+  </si>
+  <si>
+    <t>Audrain Motorspor</t>
+  </si>
+  <si>
+    <t>Liverpool FC</t>
+  </si>
+  <si>
+    <t>The Mayo Clinic</t>
+  </si>
+  <si>
+    <t>Kulicke &amp; Soffa</t>
+  </si>
+  <si>
+    <t>Insurance Claims</t>
+  </si>
+  <si>
+    <t>Entanglement</t>
+  </si>
+  <si>
+    <t>Activist Fund</t>
+  </si>
+  <si>
+    <t>SD Government</t>
+  </si>
+  <si>
+    <t>Clean Bus Solutions</t>
+  </si>
+  <si>
+    <t>Chengong</t>
+  </si>
+  <si>
+    <t>BAQSIMI</t>
+  </si>
+  <si>
+    <t>Advanced Ocean Systems</t>
+  </si>
+  <si>
+    <t>Safeway</t>
+  </si>
+  <si>
+    <t>Dogness (Intl)</t>
+  </si>
+  <si>
+    <t>Core &amp; Main Stock</t>
+  </si>
+  <si>
+    <t>Florence Copper</t>
+  </si>
+  <si>
+    <t>Investment-Grade Global Marine Operator</t>
+  </si>
+  <si>
+    <t>IM8 Health Brand</t>
+  </si>
+  <si>
+    <t>eXp Realty</t>
+  </si>
+  <si>
+    <t>Perrigo Co PLC</t>
+  </si>
+  <si>
+    <t>Journeys</t>
+  </si>
+  <si>
+    <t>Little Burgundy</t>
+  </si>
+  <si>
+    <t>Journeys Global Retail Group</t>
+  </si>
+  <si>
+    <t>Meritz Securities</t>
+  </si>
+  <si>
+    <t>CoSara</t>
+  </si>
+  <si>
+    <t>News Earnings Preview</t>
+  </si>
+  <si>
+    <t>Texas Pacific Land Corp</t>
+  </si>
+  <si>
+    <t>KGI Securities</t>
+  </si>
+  <si>
+    <t>Blockchain Wire</t>
+  </si>
+  <si>
+    <t>Foreign AI Chips</t>
+  </si>
+  <si>
+    <t>State-Funded Data Centres</t>
+  </si>
+  <si>
+    <t>This High-End Burger Chain</t>
+  </si>
+  <si>
+    <t>Archer's Midnight</t>
+  </si>
+  <si>
+    <t>TON Coins</t>
+  </si>
+  <si>
+    <t>Afterpay</t>
+  </si>
+  <si>
+    <t>PayPal Pay Later</t>
+  </si>
+  <si>
+    <t>Loan officers</t>
+  </si>
+  <si>
+    <t>Kepler Weber</t>
+  </si>
+  <si>
+    <t>Trigono Capital</t>
+  </si>
+  <si>
+    <t>A-AG Holdco</t>
+  </si>
+  <si>
+    <t>Carbyne</t>
+  </si>
+  <si>
+    <t>Equitable Hldgs</t>
+  </si>
+  <si>
+    <t>American Intl Gr</t>
+  </si>
+  <si>
+    <t>Emerging Market Stocks</t>
+  </si>
+  <si>
+    <t>Albemarle Corp</t>
+  </si>
+  <si>
+    <t>analyst updates</t>
+  </si>
+  <si>
+    <t>notes offering</t>
+  </si>
+  <si>
+    <t>Eliquis</t>
+  </si>
+  <si>
+    <t>Vyndaqel</t>
+  </si>
+  <si>
+    <t>Marathon Digital Holdings</t>
+  </si>
+  <si>
+    <t>Cipher Compute</t>
+  </si>
+  <si>
+    <t>Senior Secured Notes</t>
+  </si>
+  <si>
+    <t>Barber Lake High-Performance Data Center</t>
+  </si>
+  <si>
+    <t>Hypertrophic Cardiomyopathy Society</t>
+  </si>
+  <si>
+    <t>Transcard</t>
+  </si>
+  <si>
+    <t>FlowStocks</t>
+  </si>
+  <si>
+    <t>DYT INFO</t>
+  </si>
+  <si>
+    <t>NDV-01</t>
+  </si>
+  <si>
+    <t>Marriott Intl</t>
+  </si>
+  <si>
+    <t>Dubai Holding</t>
+  </si>
+  <si>
+    <t>Nurtec ODT/Vydura</t>
+  </si>
+  <si>
+    <t>Paxlovid</t>
+  </si>
+  <si>
+    <t>Comirnaty</t>
+  </si>
+  <si>
+    <t>Peter Ballantyne Cree Nation</t>
+  </si>
+  <si>
+    <t>Government Of Saskatchewan</t>
+  </si>
+  <si>
+    <t>Archer-Daniels Midland</t>
+  </si>
+  <si>
+    <t>fast-food chains</t>
+  </si>
+  <si>
+    <t>SBA Comms</t>
+  </si>
+  <si>
+    <t>Jehoshaphat Research</t>
+  </si>
+  <si>
+    <t>Castlelake</t>
+  </si>
+  <si>
+    <t>Biopharmaceutical Manufacturing Preparedness Consortium</t>
+  </si>
+  <si>
+    <t>MOBY Robotics</t>
+  </si>
+  <si>
+    <t>Husky Technologies</t>
+  </si>
+  <si>
+    <t>Former Honeywell CEO's Firm</t>
+  </si>
+  <si>
+    <t>Husky</t>
+  </si>
+  <si>
+    <t>Emerson Electric Inc</t>
+  </si>
+  <si>
+    <t>Ignite Visibility</t>
+  </si>
+  <si>
+    <t>EverConnect</t>
+  </si>
+  <si>
+    <t>Beijing Xinmiao Times Technology Unit</t>
+  </si>
+  <si>
+    <t>Inspur Electronic</t>
+  </si>
+  <si>
+    <t>Bystronic</t>
+  </si>
+  <si>
+    <t>Immuneering Analyst</t>
+  </si>
+  <si>
+    <t>A Person Familiar With The Discussions</t>
+  </si>
+  <si>
+    <t>Large Drugmaker</t>
+  </si>
+  <si>
+    <t>Varec Subsidiary</t>
+  </si>
+  <si>
+    <t>Karman Space &amp; Defense</t>
+  </si>
+  <si>
+    <t>Five Axis Industries</t>
+  </si>
+  <si>
+    <t>U.S. Naval Nuclear Propulsion Program</t>
+  </si>
+  <si>
+    <t>Terrian Town</t>
+  </si>
+  <si>
+    <t>Sevita</t>
+  </si>
+  <si>
+    <t>Rodaros Industria De Rodas</t>
+  </si>
+  <si>
+    <t>Rolls-Royce SMR</t>
+  </si>
+  <si>
+    <t>HeartNexus</t>
+  </si>
+  <si>
+    <t>CoMira Diagnostics</t>
+  </si>
+  <si>
+    <t>U.S.-listed ETF</t>
+  </si>
+  <si>
+    <t>ExoTerra</t>
+  </si>
+  <si>
+    <t>Arabian Eagle Manufacturing</t>
+  </si>
+  <si>
+    <t>Arabian Eagle</t>
+  </si>
+  <si>
+    <t>Cologuard</t>
+  </si>
+  <si>
+    <t>Obe-cel</t>
+  </si>
+  <si>
+    <t>Cyncado Therapeutics</t>
+  </si>
+  <si>
+    <t>International Sanctions</t>
+  </si>
+  <si>
+    <t>Rigs Odin</t>
+  </si>
+  <si>
+    <t>Rigs Hild</t>
+  </si>
+  <si>
+    <t>Wes Levitt</t>
+  </si>
+  <si>
+    <t>American College Of Gastroenterology</t>
+  </si>
+  <si>
+    <t>Voquezna Tablets For Gerd</t>
+  </si>
+  <si>
+    <t>Krystal Restaurants</t>
+  </si>
+  <si>
+    <t>Valcourt</t>
+  </si>
+  <si>
+    <t>Connecticut's Utility Overhaul</t>
+  </si>
+  <si>
+    <t>European Retailer</t>
+  </si>
+  <si>
+    <t>Morpheus AI</t>
+  </si>
+  <si>
+    <t>MKS Stock</t>
+  </si>
+  <si>
+    <t>TT-4</t>
+  </si>
+  <si>
+    <t>mesothelioma</t>
+  </si>
+  <si>
+    <t>GAMEE</t>
+  </si>
+  <si>
+    <t>Animoca Brands</t>
+  </si>
+  <si>
+    <t>symbol</t>
   </si>
   <si>
     <t>org</t>
   </si>
   <si>
+    <t>event</t>
+  </si>
+  <si>
     <t>product</t>
   </si>
   <si>
+    <t>fund</t>
+  </si>
+  <si>
+    <t>platform</t>
+  </si>
+  <si>
+    <t>executive</t>
+  </si>
+  <si>
     <t>person</t>
   </si>
   <si>
+    <t>other</t>
+  </si>
+  <si>
     <t>source</t>
   </si>
   <si>
-    <t>platform</t>
+    <t>program</t>
+  </si>
+  <si>
+    <t>macro</t>
+  </si>
+  <si>
+    <t>disease</t>
+  </si>
+  <si>
+    <t>target</t>
+  </si>
+  <si>
+    <t>partner</t>
+  </si>
+  <si>
+    <t>rater</t>
+  </si>
+  <si>
+    <t>issuer</t>
+  </si>
+  <si>
+    <t>plaintiff</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>joint_venture</t>
+  </si>
+  <si>
+    <t>distributor</t>
+  </si>
+  <si>
+    <t>newly-created organization</t>
+  </si>
+  <si>
+    <t>acquirer</t>
+  </si>
+  <si>
+    <t>supplier</t>
+  </si>
+  <si>
+    <t>defendant</t>
+  </si>
+  <si>
+    <t>competitor</t>
+  </si>
+  <si>
+    <t>rated</t>
+  </si>
+  <si>
+    <t>regulator</t>
   </si>
   <si>
     <t>discussion_hub</t>
-  </si>
-  <si>
-    <t>other</t>
-  </si>
-  <si>
-    <t>rated</t>
-  </si>
-  <si>
-    <t>target</t>
-  </si>
-  <si>
-    <t>acquirer</t>
-  </si>
-  <si>
-    <t>executive</t>
-  </si>
-  <si>
-    <t>partner</t>
-  </si>
-  <si>
-    <t>issuer</t>
-  </si>
-  <si>
-    <t>supplier</t>
-  </si>
-  <si>
-    <t>licensed</t>
   </si>
 </sst>
 </file>
@@ -575,7 +839,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:C126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -597,10 +861,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" t="s">
-        <v>60</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -608,10 +869,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C3" t="s">
-        <v>61</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -619,10 +877,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" t="s">
-        <v>61</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -630,10 +885,10 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -641,10 +896,10 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>128</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -652,10 +907,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="C7" t="s">
-        <v>59</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -663,10 +918,10 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>128</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -674,10 +929,10 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>128</v>
       </c>
       <c r="C9" t="s">
-        <v>63</v>
+        <v>142</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -685,10 +940,10 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="C10" t="s">
-        <v>64</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -696,10 +951,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -707,10 +962,10 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>128</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -718,10 +973,10 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>140</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -729,10 +984,10 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="C14" t="s">
-        <v>64</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -740,10 +995,10 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>53</v>
+        <v>131</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -751,10 +1006,10 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>56</v>
+        <v>128</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>145</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -762,10 +1017,10 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="C17" t="s">
-        <v>62</v>
+        <v>146</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -773,10 +1028,10 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="C18" t="s">
-        <v>64</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -784,10 +1039,10 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -795,10 +1050,10 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="C20" t="s">
-        <v>65</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -806,10 +1061,10 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -817,10 +1072,10 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>143</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -828,10 +1083,10 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>130</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>140</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -839,10 +1094,10 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="C24" t="s">
-        <v>65</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -850,10 +1105,10 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -861,10 +1116,10 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="C26" t="s">
-        <v>61</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -872,10 +1127,10 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>128</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -883,10 +1138,10 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>55</v>
+        <v>128</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -894,10 +1149,10 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="C29" t="s">
-        <v>61</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -905,10 +1160,10 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>128</v>
       </c>
       <c r="C30" t="s">
-        <v>61</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -916,10 +1171,10 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -927,10 +1182,10 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>57</v>
+        <v>128</v>
       </c>
       <c r="C32" t="s">
-        <v>58</v>
+        <v>149</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -938,10 +1193,10 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="C33" t="s">
-        <v>64</v>
+        <v>140</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -949,10 +1204,10 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>130</v>
       </c>
       <c r="C34" t="s">
-        <v>54</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -960,10 +1215,10 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>58</v>
+        <v>128</v>
       </c>
       <c r="C35" t="s">
-        <v>58</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -971,10 +1226,10 @@
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>54</v>
+        <v>131</v>
       </c>
       <c r="C36" t="s">
-        <v>59</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -982,10 +1237,10 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>54</v>
+        <v>128</v>
       </c>
       <c r="C37" t="s">
-        <v>59</v>
+        <v>140</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -993,10 +1248,10 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>54</v>
+        <v>130</v>
       </c>
       <c r="C38" t="s">
-        <v>61</v>
+        <v>140</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -1004,10 +1259,10 @@
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>53</v>
+        <v>132</v>
       </c>
       <c r="C39" t="s">
-        <v>60</v>
+        <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1015,10 +1270,10 @@
         <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>54</v>
+        <v>128</v>
       </c>
       <c r="C40" t="s">
-        <v>61</v>
+        <v>140</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -1026,10 +1281,10 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="C41" t="s">
-        <v>65</v>
+        <v>140</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1037,10 +1292,10 @@
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>53</v>
+        <v>130</v>
       </c>
       <c r="C42" t="s">
-        <v>64</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -1048,10 +1303,10 @@
         <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="C43" t="s">
-        <v>65</v>
+        <v>150</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1059,10 +1314,10 @@
         <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="C44" t="s">
-        <v>61</v>
+        <v>150</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -1070,10 +1325,10 @@
         <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>53</v>
+        <v>133</v>
       </c>
       <c r="C45" t="s">
-        <v>61</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1081,10 +1336,10 @@
         <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>53</v>
+        <v>134</v>
       </c>
       <c r="C46" t="s">
-        <v>62</v>
+        <v>142</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -1092,10 +1347,10 @@
         <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>54</v>
+        <v>128</v>
       </c>
       <c r="C47" t="s">
-        <v>54</v>
+        <v>140</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1103,10 +1358,10 @@
         <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>53</v>
+        <v>128</v>
       </c>
       <c r="C48" t="s">
-        <v>61</v>
+        <v>149</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -1114,10 +1369,10 @@
         <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>54</v>
+        <v>128</v>
       </c>
       <c r="C49" t="s">
-        <v>67</v>
+        <v>140</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -1125,10 +1380,10 @@
         <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>59</v>
+        <v>128</v>
       </c>
       <c r="C50" t="s">
-        <v>62</v>
+        <v>143</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -1136,10 +1391,835 @@
         <v>52</v>
       </c>
       <c r="B51" t="s">
+        <v>128</v>
+      </c>
+      <c r="C51" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3">
+      <c r="A52" t="s">
         <v>53</v>
       </c>
-      <c r="C51" t="s">
+      <c r="B52" t="s">
+        <v>135</v>
+      </c>
+      <c r="C52" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3">
+      <c r="A53" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53" t="s">
+        <v>128</v>
+      </c>
+      <c r="C53" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3">
+      <c r="A54" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54" t="s">
+        <v>136</v>
+      </c>
+      <c r="C54" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" t="s">
+        <v>56</v>
+      </c>
+      <c r="B55" t="s">
+        <v>135</v>
+      </c>
+      <c r="C55" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3">
+      <c r="A56" t="s">
+        <v>57</v>
+      </c>
+      <c r="B56" t="s">
+        <v>130</v>
+      </c>
+      <c r="C56" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3">
+      <c r="A57" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" t="s">
+        <v>130</v>
+      </c>
+      <c r="C57" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" t="s">
+        <v>59</v>
+      </c>
+      <c r="B58" t="s">
+        <v>128</v>
+      </c>
+      <c r="C58" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3">
+      <c r="A59" t="s">
+        <v>60</v>
+      </c>
+      <c r="B59" t="s">
+        <v>128</v>
+      </c>
+      <c r="C59" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3">
+      <c r="A60" t="s">
+        <v>61</v>
+      </c>
+      <c r="B60" t="s">
+        <v>130</v>
+      </c>
+      <c r="C60" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3">
+      <c r="A61" t="s">
         <v>62</v>
+      </c>
+      <c r="B61" t="s">
+        <v>130</v>
+      </c>
+      <c r="C61" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3">
+      <c r="A62" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" t="s">
+        <v>128</v>
+      </c>
+      <c r="C62" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>64</v>
+      </c>
+      <c r="B63" t="s">
+        <v>128</v>
+      </c>
+      <c r="C63" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64" t="s">
+        <v>132</v>
+      </c>
+      <c r="C64" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65" t="s">
+        <v>128</v>
+      </c>
+      <c r="C65" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>67</v>
+      </c>
+      <c r="B66" t="s">
+        <v>130</v>
+      </c>
+      <c r="C66" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>68</v>
+      </c>
+      <c r="B67" t="s">
+        <v>128</v>
+      </c>
+      <c r="C67" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>69</v>
+      </c>
+      <c r="B68" t="s">
+        <v>128</v>
+      </c>
+      <c r="C68" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>70</v>
+      </c>
+      <c r="B69" t="s">
+        <v>130</v>
+      </c>
+      <c r="C69" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>71</v>
+      </c>
+      <c r="B70" t="s">
+        <v>130</v>
+      </c>
+      <c r="C70" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>72</v>
+      </c>
+      <c r="B71" t="s">
+        <v>130</v>
+      </c>
+      <c r="C71" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>73</v>
+      </c>
+      <c r="B72" t="s">
+        <v>128</v>
+      </c>
+      <c r="C72" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>74</v>
+      </c>
+      <c r="B73" t="s">
+        <v>128</v>
+      </c>
+      <c r="C73" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" t="s">
+        <v>75</v>
+      </c>
+      <c r="B74" t="s">
+        <v>128</v>
+      </c>
+      <c r="C74" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>76</v>
+      </c>
+      <c r="B75" t="s">
+        <v>135</v>
+      </c>
+      <c r="C75" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" t="s">
+        <v>77</v>
+      </c>
+      <c r="B76" t="s">
+        <v>128</v>
+      </c>
+      <c r="C76" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" t="s">
+        <v>78</v>
+      </c>
+      <c r="B77" t="s">
+        <v>128</v>
+      </c>
+      <c r="C77" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78" t="s">
+        <v>128</v>
+      </c>
+      <c r="C78" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" t="s">
+        <v>80</v>
+      </c>
+      <c r="B79" t="s">
+        <v>128</v>
+      </c>
+      <c r="C79" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" t="s">
+        <v>81</v>
+      </c>
+      <c r="B80" t="s">
+        <v>128</v>
+      </c>
+      <c r="C80" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" t="s">
+        <v>82</v>
+      </c>
+      <c r="B81" t="s">
+        <v>128</v>
+      </c>
+      <c r="C81" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" t="s">
+        <v>83</v>
+      </c>
+      <c r="B82" t="s">
+        <v>128</v>
+      </c>
+      <c r="C82" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" t="s">
+        <v>84</v>
+      </c>
+      <c r="B83" t="s">
+        <v>128</v>
+      </c>
+      <c r="C83" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" t="s">
+        <v>85</v>
+      </c>
+      <c r="B84" t="s">
+        <v>128</v>
+      </c>
+      <c r="C84" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" t="s">
+        <v>86</v>
+      </c>
+      <c r="B85" t="s">
+        <v>128</v>
+      </c>
+      <c r="C85" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" t="s">
+        <v>87</v>
+      </c>
+      <c r="B86" t="s">
+        <v>130</v>
+      </c>
+      <c r="C86" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" t="s">
+        <v>88</v>
+      </c>
+      <c r="B87" t="s">
+        <v>128</v>
+      </c>
+      <c r="C87" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" t="s">
+        <v>89</v>
+      </c>
+      <c r="B88" t="s">
+        <v>128</v>
+      </c>
+      <c r="C88" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" t="s">
+        <v>90</v>
+      </c>
+      <c r="B89" t="s">
+        <v>128</v>
+      </c>
+      <c r="C89" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" t="s">
+        <v>91</v>
+      </c>
+      <c r="B90" t="s">
+        <v>134</v>
+      </c>
+      <c r="C90" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" t="s">
+        <v>92</v>
+      </c>
+      <c r="B91" t="s">
+        <v>134</v>
+      </c>
+      <c r="C91" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" t="s">
+        <v>93</v>
+      </c>
+      <c r="B92" t="s">
+        <v>128</v>
+      </c>
+      <c r="C92" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" t="s">
+        <v>94</v>
+      </c>
+      <c r="B93" t="s">
+        <v>128</v>
+      </c>
+      <c r="C93" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" t="s">
+        <v>95</v>
+      </c>
+      <c r="B94" t="s">
+        <v>128</v>
+      </c>
+      <c r="C94" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" t="s">
+        <v>96</v>
+      </c>
+      <c r="B95" t="s">
+        <v>128</v>
+      </c>
+      <c r="C95" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" t="s">
+        <v>97</v>
+      </c>
+      <c r="B96" t="s">
+        <v>137</v>
+      </c>
+      <c r="C96" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3">
+      <c r="A97" t="s">
+        <v>98</v>
+      </c>
+      <c r="B97" t="s">
+        <v>128</v>
+      </c>
+      <c r="C97" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" t="s">
+        <v>3</v>
+      </c>
+      <c r="B98" t="s">
+        <v>128</v>
+      </c>
+      <c r="C98" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3">
+      <c r="A99" t="s">
+        <v>99</v>
+      </c>
+      <c r="B99" t="s">
+        <v>128</v>
+      </c>
+      <c r="C99" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3">
+      <c r="A100" t="s">
+        <v>100</v>
+      </c>
+      <c r="B100" t="s">
+        <v>128</v>
+      </c>
+      <c r="C100" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3">
+      <c r="A101" t="s">
+        <v>101</v>
+      </c>
+      <c r="B101" t="s">
+        <v>130</v>
+      </c>
+      <c r="C101" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3">
+      <c r="A102" t="s">
+        <v>102</v>
+      </c>
+      <c r="B102" t="s">
+        <v>128</v>
+      </c>
+      <c r="C102" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3">
+      <c r="A103" t="s">
+        <v>103</v>
+      </c>
+      <c r="B103" t="s">
+        <v>128</v>
+      </c>
+      <c r="C103" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3">
+      <c r="A104" t="s">
+        <v>104</v>
+      </c>
+      <c r="B104" t="s">
+        <v>130</v>
+      </c>
+      <c r="C104" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" t="s">
+        <v>105</v>
+      </c>
+      <c r="B105" t="s">
+        <v>128</v>
+      </c>
+      <c r="C105" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3">
+      <c r="A106" t="s">
+        <v>106</v>
+      </c>
+      <c r="B106" t="s">
+        <v>128</v>
+      </c>
+      <c r="C106" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3">
+      <c r="A107" t="s">
+        <v>107</v>
+      </c>
+      <c r="B107" t="s">
+        <v>128</v>
+      </c>
+      <c r="C107" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3">
+      <c r="A108" t="s">
+        <v>108</v>
+      </c>
+      <c r="B108" t="s">
+        <v>130</v>
+      </c>
+      <c r="C108" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3">
+      <c r="A109" t="s">
+        <v>109</v>
+      </c>
+      <c r="B109" t="s">
+        <v>130</v>
+      </c>
+      <c r="C109" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3">
+      <c r="A110" t="s">
+        <v>110</v>
+      </c>
+      <c r="B110" t="s">
+        <v>128</v>
+      </c>
+      <c r="C110" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3">
+      <c r="A111" t="s">
+        <v>111</v>
+      </c>
+      <c r="B111" t="s">
+        <v>138</v>
+      </c>
+      <c r="C111" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3">
+      <c r="A112" t="s">
+        <v>112</v>
+      </c>
+      <c r="B112" t="s">
+        <v>130</v>
+      </c>
+      <c r="C112" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" t="s">
+        <v>113</v>
+      </c>
+      <c r="B113" t="s">
+        <v>130</v>
+      </c>
+      <c r="C113" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" t="s">
+        <v>114</v>
+      </c>
+      <c r="B114" t="s">
+        <v>134</v>
+      </c>
+      <c r="C114" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" t="s">
+        <v>115</v>
+      </c>
+      <c r="B115" t="s">
+        <v>128</v>
+      </c>
+      <c r="C115" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" t="s">
+        <v>116</v>
+      </c>
+      <c r="B116" t="s">
+        <v>130</v>
+      </c>
+      <c r="C116" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" t="s">
+        <v>117</v>
+      </c>
+      <c r="B117" t="s">
+        <v>128</v>
+      </c>
+      <c r="C117" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" t="s">
+        <v>118</v>
+      </c>
+      <c r="B118" t="s">
+        <v>128</v>
+      </c>
+      <c r="C118" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" t="s">
+        <v>119</v>
+      </c>
+      <c r="B119" t="s">
+        <v>138</v>
+      </c>
+      <c r="C119" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" t="s">
+        <v>120</v>
+      </c>
+      <c r="B120" t="s">
+        <v>128</v>
+      </c>
+      <c r="C120" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" t="s">
+        <v>121</v>
+      </c>
+      <c r="B121" t="s">
+        <v>128</v>
+      </c>
+      <c r="C121" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" t="s">
+        <v>122</v>
+      </c>
+      <c r="B122" t="s">
+        <v>135</v>
+      </c>
+      <c r="C122" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" t="s">
+        <v>123</v>
+      </c>
+      <c r="B123" t="s">
+        <v>130</v>
+      </c>
+      <c r="C123" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" t="s">
+        <v>124</v>
+      </c>
+      <c r="B124" t="s">
+        <v>139</v>
+      </c>
+      <c r="C124" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" t="s">
+        <v>125</v>
+      </c>
+      <c r="B125" t="s">
+        <v>128</v>
+      </c>
+      <c r="C125" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" t="s">
+        <v>126</v>
+      </c>
+      <c r="B126" t="s">
+        <v>128</v>
+      </c>
+      <c r="C126" t="s">
+        <v>141</v>
       </c>
     </row>
   </sheetData>

</xml_diff>